<commit_message>
update file and task
</commit_message>
<xml_diff>
--- a/dev_doc/Management/项目计划甘特图.xlsx
+++ b/dev_doc/Management/项目计划甘特图.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22488" windowHeight="9347" tabRatio="634"/>
+    <workbookView windowWidth="22488" windowHeight="9347" tabRatio="634" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="甘特图" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="149">
   <si>
     <t>任务
 序号</t>
@@ -841,16 +841,34 @@
     <t>120人日</t>
   </si>
   <si>
-    <t>徐传旭，刘文佳，张涵，张莹</t>
+    <t>陈子源，胡品爵，董哲，杜少恒，徐传旭，张涵，张莹，刘文佳</t>
+  </si>
+  <si>
+    <t>5人日</t>
+  </si>
+  <si>
+    <t>刘文佳</t>
+  </si>
+  <si>
+    <t>张涵，董哲</t>
+  </si>
+  <si>
+    <t>张莹，胡品爵，杜少恒</t>
+  </si>
+  <si>
+    <t>张莹，徐传旭</t>
   </si>
   <si>
     <t>1人日</t>
   </si>
   <si>
-    <t>刘文佳</t>
+    <t>董哲，刘文佳，王智超，陈子源，杜少恒</t>
   </si>
   <si>
-    <t>张涵</t>
+    <t>2人日</t>
+  </si>
+  <si>
+    <t>刘文佳，王智超，董哲，杜少恒</t>
   </si>
   <si>
     <t>80人日</t>
@@ -862,28 +880,34 @@
     <t>胡品爵，董哲，杜少恒，王智超，徐传旭，张涵，张建鹏，张莹，刘文佳</t>
   </si>
   <si>
+    <t>胡品爵，董哲，杜少恒，王智超，张建鹏</t>
+  </si>
+  <si>
     <t>20197/2</t>
+  </si>
+  <si>
+    <t>张涵</t>
   </si>
   <si>
     <t>2工作日</t>
   </si>
   <si>
-    <t>胡品爵，董哲，杜少恒，王智超，张建鹏</t>
+    <t>?</t>
   </si>
   <si>
-    <t>徐传旭，张莹</t>
+    <t>张涵，陈子源，张莹</t>
   </si>
   <si>
-    <t>?</t>
+    <t>陈子源，张莹</t>
+  </si>
+  <si>
+    <t>张涵，徐传旭</t>
   </si>
   <si>
     <t>3人日</t>
   </si>
   <si>
     <t>20人日</t>
-  </si>
-  <si>
-    <t>2人日</t>
   </si>
   <si>
     <t>18人日</t>
@@ -901,14 +925,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="d"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
     <numFmt numFmtId="177" formatCode="0&quot; 人日&quot;"/>
-    <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="179" formatCode="0&quot; 工作日&quot;"/>
-    <numFmt numFmtId="180" formatCode="yyyy&quot;年&quot;m&quot;月&quot;;@"/>
+    <numFmt numFmtId="178" formatCode="0&quot; 工作日&quot;"/>
+    <numFmt numFmtId="179" formatCode="yyyy&quot;年&quot;m&quot;月&quot;;@"/>
+    <numFmt numFmtId="180" formatCode="d"/>
     <numFmt numFmtId="181" formatCode="[$-804]aaa;@"/>
   </numFmts>
   <fonts count="29">
@@ -970,17 +994,18 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1000,23 +1025,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1030,23 +1063,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1062,15 +1086,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1084,13 +1114,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1099,15 +1122,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1146,13 +1170,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1164,7 +1188,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1176,67 +1236,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1254,7 +1254,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1266,7 +1278,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1278,37 +1296,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1466,6 +1490,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1483,9 +1525,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1501,41 +1560,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1569,10 +1593,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1581,19 +1605,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1602,112 +1626,112 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1716,7 +1740,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1725,7 +1749,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1737,34 +1761,34 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1773,7 +1797,7 @@
     <xf numFmtId="177" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1791,16 +1815,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1836,7 +1860,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12462,12 +12486,12 @@
   <sheetPr/>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M46" sqref="M46"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
@@ -14204,8 +14228,8 @@
   <sheetPr/>
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
@@ -14419,7 +14443,7 @@
       </c>
       <c r="I7" s="20">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -14439,7 +14463,7 @@
         <v>43647</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>24</v>
@@ -14450,7 +14474,7 @@
       </c>
       <c r="I8" s="20">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14470,7 +14494,7 @@
         <v>43647</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>24</v>
@@ -14480,7 +14504,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -14499,7 +14523,9 @@
       <c r="E10" s="13">
         <v>43647</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>125</v>
+      </c>
       <c r="G10" s="14" t="s">
         <v>24</v>
       </c>
@@ -14508,7 +14534,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14540,25 +14566,24 @@
       <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="9">
         <v>43648</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="9">
         <v>43648</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="11">
         <f>NETWORKDAYS.INTL(D12,E12,"0000000")</f>
         <v>1</v>
       </c>
-      <c r="I12" s="20">
-        <f>H12*(LEN(F12)-LEN(SUBSTITUTE(F12,"，",""))+1)</f>
-        <v>1</v>
+      <c r="I12" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -14578,7 +14603,7 @@
         <v>43648</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>24</v>
@@ -14589,7 +14614,7 @@
       </c>
       <c r="I13" s="20">
         <f>H13*(LEN(F13)-LEN(SUBSTITUTE(F13,"，",""))+1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -14608,9 +14633,8 @@
       <c r="E14" s="13">
         <v>43648</v>
       </c>
-      <c r="F14" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F14" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>24</v>
@@ -14670,7 +14694,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -14700,7 +14724,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -14781,7 +14805,7 @@
         <v>43650</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>24</v>
@@ -14810,9 +14834,8 @@
       <c r="E21" s="13">
         <v>43648</v>
       </c>
-      <c r="F21" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F21" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>24</v>
@@ -14836,20 +14859,19 @@
         <v>36</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E22" s="13">
         <v>43649</v>
       </c>
-      <c r="F22" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F22" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>24</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="I22" s="20">
         <v>2</v>
@@ -14871,9 +14893,8 @@
       <c r="E23" s="13">
         <v>43649</v>
       </c>
-      <c r="F23" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F23" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>24</v>
@@ -14903,7 +14924,7 @@
         <v>43650</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>24</v>
@@ -14932,9 +14953,8 @@
       <c r="E25" s="13">
         <v>43650</v>
       </c>
-      <c r="F25" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F25" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>24</v>
@@ -14964,7 +14984,7 @@
         <v>43650</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>24</v>
@@ -14993,9 +15013,8 @@
       <c r="E27" s="13">
         <v>43650</v>
       </c>
-      <c r="F27" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F27" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>24</v>
@@ -15024,9 +15043,8 @@
       <c r="E28" s="13">
         <v>43650</v>
       </c>
-      <c r="F28" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F28" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>24</v>
@@ -15055,9 +15073,8 @@
       <c r="E29" s="13">
         <v>43650</v>
       </c>
-      <c r="F29" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F29" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>24</v>
@@ -15168,7 +15185,7 @@
         <v>43653</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>24</v>
@@ -15197,9 +15214,8 @@
       <c r="E34" s="13">
         <v>43651</v>
       </c>
-      <c r="F34" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F34" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>24</v>
@@ -15228,9 +15244,8 @@
       <c r="E35" s="13">
         <v>43651</v>
       </c>
-      <c r="F35" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F35" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G35" s="14" t="s">
         <v>24</v>
@@ -15259,9 +15274,8 @@
       <c r="E36" s="13">
         <v>43651</v>
       </c>
-      <c r="F36" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F36" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>24</v>
@@ -15291,7 +15305,7 @@
         <v>43653</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>24</v>
@@ -15320,9 +15334,8 @@
       <c r="E38" s="13">
         <v>43653</v>
       </c>
-      <c r="F38" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F38" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="G38" s="14" t="s">
         <v>24</v>
@@ -15352,7 +15365,7 @@
         <v>43653</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>24</v>
@@ -15381,9 +15394,8 @@
       <c r="E40" s="13">
         <v>43653</v>
       </c>
-      <c r="F40" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F40" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="G40" s="14" t="s">
         <v>24</v>
@@ -15412,9 +15424,8 @@
       <c r="E41" s="13">
         <v>43653</v>
       </c>
-      <c r="F41" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F41" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>24</v>
@@ -15443,9 +15454,8 @@
       <c r="E42" s="13">
         <v>43653</v>
       </c>
-      <c r="F42" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F42" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>24</v>
@@ -15455,7 +15465,7 @@
         <v>3</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -15505,7 +15515,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -15536,7 +15546,7 @@
         <v>2</v>
       </c>
       <c r="I45" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -15556,7 +15566,7 @@
         <v>43655</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>24</v>
@@ -15566,7 +15576,7 @@
         <v>2</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -15585,9 +15595,8 @@
       <c r="E47" s="13">
         <v>43654</v>
       </c>
-      <c r="F47" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F47" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="G47" s="14" t="s">
         <v>24</v>
@@ -15597,7 +15606,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -15616,9 +15625,8 @@
       <c r="E48" s="13">
         <v>43654</v>
       </c>
-      <c r="F48" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F48" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="G48" s="14" t="s">
         <v>24</v>
@@ -15628,7 +15636,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -15647,9 +15655,8 @@
       <c r="E49" s="13">
         <v>43654</v>
       </c>
-      <c r="F49" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F49" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="G49" s="14" t="s">
         <v>24</v>
@@ -15659,7 +15666,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -15679,7 +15686,7 @@
         <v>43655</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G50" s="14" t="s">
         <v>24</v>
@@ -15708,9 +15715,8 @@
       <c r="E51" s="13">
         <v>43655</v>
       </c>
-      <c r="F51" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F51" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="G51" s="14" t="s">
         <v>24</v>
@@ -15720,7 +15726,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -15740,7 +15746,7 @@
         <v>43655</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>24</v>
@@ -15750,7 +15756,7 @@
         <v>2</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -15769,9 +15775,8 @@
       <c r="E53" s="13">
         <v>43655</v>
       </c>
-      <c r="F53" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F53" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>24</v>
@@ -15781,7 +15786,7 @@
         <v>2</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -15800,9 +15805,8 @@
       <c r="E54" s="13">
         <v>43655</v>
       </c>
-      <c r="F54" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F54" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>24</v>
@@ -15812,7 +15816,7 @@
         <v>2</v>
       </c>
       <c r="I54" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -15831,9 +15835,8 @@
       <c r="E55" s="13">
         <v>43655</v>
       </c>
-      <c r="F55" s="14" t="e">
-        <f>甘特图!#REF!</f>
-        <v>#REF!</v>
+      <c r="F55" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>24</v>
@@ -15843,7 +15846,7 @@
         <v>2</v>
       </c>
       <c r="I55" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -15912,7 +15915,7 @@
         <v>3</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -15943,7 +15946,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -15974,7 +15977,7 @@
         <v>2</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -16005,7 +16008,7 @@
         <v>2</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -16036,7 +16039,7 @@
         <v>2</v>
       </c>
       <c r="I62" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -16065,7 +16068,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:9">

</xml_diff>